<commit_message>
branch02.txt add new message
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="1">
   <si>
     <t>PayMB</t>
     <phoneticPr fontId="5"/>
@@ -425,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E7"/>
+  <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E7"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18"/>
@@ -517,6 +518,82 @@
         <v>47195</v>
       </c>
     </row>
+    <row r="11" spans="2:5">
+      <c r="B11" s="1">
+        <v>47146</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5">
+      <c r="B12" s="2">
+        <v>47145</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5">
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5">
+      <c r="B14" s="4">
+        <v>47195</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5">
+      <c r="B15" s="4">
+        <v>47195</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5">
+      <c r="B16" s="4">
+        <v>47195</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:B8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18"/>
+  <sheetData>
+    <row r="3" spans="2:2">
+      <c r="B3" s="1">
+        <v>47146</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="2">
+        <v>47145</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" s="4">
+        <v>47195</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2">
+      <c r="B7" s="4">
+        <v>47195</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" s="4">
+        <v>47195</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>